<commit_message>
Add GPU enabled version and update test results
</commit_message>
<xml_diff>
--- a/Mars/Results experiment.xlsx
+++ b/Mars/Results experiment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OMSA\ISyE6748_practicum_publish\Mars\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC57F9A7-ED04-488B-8E46-026F33649C29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{758BE938-72D6-4EE8-B1B9-9A56D07B1052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{E4D7315C-30FB-4E3F-97F4-414471C9F41B}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="111">
   <si>
     <t>Rank (x, y, z)</t>
   </si>
@@ -270,15 +270,6 @@
     <t>35 at 0.98</t>
   </si>
   <si>
-    <t>Autoencoder and OC-SVM</t>
-  </si>
-  <si>
-    <t>Factor 20 (bottleneck 16)</t>
-  </si>
-  <si>
-    <t>50 at 0.66</t>
-  </si>
-  <si>
     <t>Labels</t>
   </si>
   <si>
@@ -340,6 +331,45 @@
   </si>
   <si>
     <t>(20, 20)</t>
+  </si>
+  <si>
+    <t>55 at 0.8</t>
+  </si>
+  <si>
+    <t>NO Decomposition</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Params</t>
+  </si>
+  <si>
+    <t>{'gamma': 'scale', 'kernel': 'poly', 'nu': 0.05}</t>
+  </si>
+  <si>
+    <t>{'contamination': 0.05, 'max_features': 1.0, 'max_samples': 1.0, 'n_estimators': 50}</t>
+  </si>
+  <si>
+    <t>Autoencoder with oc svm</t>
+  </si>
+  <si>
+    <t>Factor=2, bottleneck=16</t>
+  </si>
+  <si>
+    <t>no difference seen changing factors and bottleneck values</t>
+  </si>
+  <si>
+    <t>No Decomposition</t>
+  </si>
+  <si>
+    <t>Autoencoder with oc-svm</t>
+  </si>
+  <si>
+    <t>Run time</t>
+  </si>
+  <si>
+    <t>Autoencoder and OC-SVM: Factor 20 (bottleneck 16)</t>
   </si>
 </sst>
 </file>
@@ -375,9 +405,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -712,15 +741,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E08DC109-0DFE-425C-811D-898250066C7D}">
-  <dimension ref="A1:F93"/>
+  <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="F82" sqref="F82"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.109375" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" customWidth="1"/>
     <col min="3" max="3" width="22.21875" customWidth="1"/>
     <col min="4" max="4" width="17.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.5546875" customWidth="1"/>
@@ -1256,7 +1285,7 @@
       <c r="A68" t="s">
         <v>67</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="C68" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1276,7 +1305,7 @@
         <v>75</v>
       </c>
       <c r="F72" t="s">
-        <v>77</v>
+        <v>110</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -1293,7 +1322,7 @@
         <v>1</v>
       </c>
       <c r="F73" t="s">
-        <v>78</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
@@ -1327,7 +1356,7 @@
         <v>0.44</v>
       </c>
       <c r="F75">
-        <v>0.6</v>
+        <v>0.56000000000000005</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
@@ -1344,7 +1373,7 @@
         <v>0.46</v>
       </c>
       <c r="F76">
-        <v>0.36</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
@@ -1378,7 +1407,7 @@
         <v>0.92</v>
       </c>
       <c r="F78">
-        <v>0.6</v>
+        <v>0.56000000000000005</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -1395,7 +1424,7 @@
         <v>0.98</v>
       </c>
       <c r="F79">
-        <v>0.36</v>
+        <v>0.56000000000000005</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
@@ -1412,7 +1441,7 @@
         <v>0.96</v>
       </c>
       <c r="F80">
-        <v>0.62</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
@@ -1429,7 +1458,7 @@
         <v>0.96</v>
       </c>
       <c r="F81">
-        <v>0.62</v>
+        <v>0.56000000000000005</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
@@ -1446,7 +1475,7 @@
         <v>0.96</v>
       </c>
       <c r="F82">
-        <v>0.66</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
@@ -1463,7 +1492,7 @@
         <v>0.9</v>
       </c>
       <c r="F83">
-        <v>0.62</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -1480,7 +1509,7 @@
         <v>0.92</v>
       </c>
       <c r="F84">
-        <v>0.6</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
@@ -1497,7 +1526,7 @@
         <v>0.54</v>
       </c>
       <c r="F85">
-        <v>0.62</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
@@ -1514,7 +1543,7 @@
         <v>0.5</v>
       </c>
       <c r="F86">
-        <v>0.4</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
@@ -1531,7 +1560,7 @@
         <v>0.42</v>
       </c>
       <c r="F87">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
@@ -1548,7 +1577,7 @@
         <v>0.46</v>
       </c>
       <c r="F88">
-        <v>0.4</v>
+        <v>0.56000000000000005</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
@@ -1564,6 +1593,9 @@
       <c r="E89">
         <v>0.48</v>
       </c>
+      <c r="F89">
+        <v>0.56000000000000005</v>
+      </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B90">
@@ -1578,6 +1610,9 @@
       <c r="E90">
         <v>0.48</v>
       </c>
+      <c r="F90">
+        <v>0.46</v>
+      </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B91">
@@ -1592,6 +1627,9 @@
       <c r="E91">
         <v>0.5</v>
       </c>
+      <c r="F91">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
@@ -1607,7 +1645,67 @@
         <v>76</v>
       </c>
       <c r="F93" t="s">
-        <v>79</v>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="97" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B97" t="s">
+        <v>100</v>
+      </c>
+      <c r="C97" t="s">
+        <v>1</v>
+      </c>
+      <c r="D97" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="98" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B98" t="s">
+        <v>73</v>
+      </c>
+      <c r="C98">
+        <v>0.62</v>
+      </c>
+      <c r="D98" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="99" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B99" t="s">
+        <v>74</v>
+      </c>
+      <c r="C99">
+        <v>0.44</v>
+      </c>
+      <c r="D99" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="100" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B100" t="s">
+        <v>75</v>
+      </c>
+      <c r="C100">
+        <v>0.42</v>
+      </c>
+      <c r="D100" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="101" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B101" t="s">
+        <v>108</v>
+      </c>
+      <c r="C101">
+        <v>0.74</v>
+      </c>
+      <c r="D101" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1618,13 +1716,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43ED864E-F45D-4DB1-A622-1F4710D7B3A3}">
-  <dimension ref="A1:L53"/>
+  <dimension ref="A1:N62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -1636,7 +1737,7 @@
         <v>73</v>
       </c>
       <c r="G2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -1866,7 +1967,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
@@ -2386,12 +2487,12 @@
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
@@ -2399,12 +2500,12 @@
         <v>73</v>
       </c>
       <c r="G35" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -2439,7 +2540,7 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C37">
         <v>0.63970000000000005</v>
@@ -2474,7 +2575,7 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C38">
         <v>0.60640000000000005</v>
@@ -2509,7 +2610,7 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C39">
         <v>0.63339999999999996</v>
@@ -2544,7 +2645,7 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C40">
         <v>0.6421</v>
@@ -2579,7 +2680,7 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C41">
         <v>0.56040000000000001</v>
@@ -2614,7 +2715,7 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C42">
         <v>0.56569999999999998</v>
@@ -2649,7 +2750,7 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C43">
         <v>0.5554</v>
@@ -2684,7 +2785,7 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C44">
         <v>0.54349999999999998</v>
@@ -2719,7 +2820,7 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C45">
         <v>0.53</v>
@@ -2754,7 +2855,7 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C46">
         <v>0.53979999999999995</v>
@@ -2789,7 +2890,7 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C47">
         <v>0.61370000000000002</v>
@@ -2824,7 +2925,7 @@
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C48">
         <v>0.60950000000000004</v>
@@ -2857,9 +2958,9 @@
         <v>0.87990000000000002</v>
       </c>
     </row>
-    <row r="49" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C49">
         <v>0.52990000000000004</v>
@@ -2892,9 +2993,9 @@
         <v>0.96930000000000005</v>
       </c>
     </row>
-    <row r="50" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C50">
         <v>0.53769999999999996</v>
@@ -2927,9 +3028,9 @@
         <v>0.93569999999999998</v>
       </c>
     </row>
-    <row r="51" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C51">
         <v>0.60609999999999997</v>
@@ -2962,9 +3063,9 @@
         <v>0.85470000000000002</v>
       </c>
     </row>
-    <row r="52" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C52">
         <v>0.59540000000000004</v>
@@ -2997,7 +3098,7 @@
         <v>0.82240000000000002</v>
       </c>
     </row>
-    <row r="53" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>67</v>
       </c>
@@ -3040,6 +3141,164 @@
       <c r="L53">
         <f t="shared" si="3"/>
         <v>0.97019999999999995</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G57" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B58" t="s">
+        <v>100</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <v>1</v>
+      </c>
+      <c r="F58">
+        <v>2</v>
+      </c>
+      <c r="G58">
+        <v>3</v>
+      </c>
+      <c r="H58">
+        <v>4</v>
+      </c>
+      <c r="I58">
+        <v>5</v>
+      </c>
+      <c r="J58">
+        <v>6</v>
+      </c>
+      <c r="K58">
+        <v>7</v>
+      </c>
+      <c r="L58">
+        <v>8</v>
+      </c>
+      <c r="M58">
+        <v>9</v>
+      </c>
+      <c r="N58" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B59" t="s">
+        <v>73</v>
+      </c>
+      <c r="D59">
+        <v>0.93200000000000005</v>
+      </c>
+      <c r="E59">
+        <v>0.97299999999999998</v>
+      </c>
+      <c r="F59">
+        <v>0.9</v>
+      </c>
+      <c r="G59">
+        <v>0.93799999999999994</v>
+      </c>
+      <c r="H59">
+        <v>0.90100000000000002</v>
+      </c>
+      <c r="I59">
+        <v>0.90259999999999996</v>
+      </c>
+      <c r="J59">
+        <v>0.9</v>
+      </c>
+      <c r="K59">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="L59">
+        <v>0.92100000000000004</v>
+      </c>
+      <c r="M59">
+        <v>0.96499999999999997</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B60" t="s">
+        <v>74</v>
+      </c>
+      <c r="D60">
+        <v>0.60840000000000005</v>
+      </c>
+      <c r="E60">
+        <v>0.91749999999999998</v>
+      </c>
+      <c r="F60">
+        <v>0.54410000000000003</v>
+      </c>
+      <c r="G60">
+        <v>0.82199999999999995</v>
+      </c>
+      <c r="H60">
+        <v>0.62690000000000001</v>
+      </c>
+      <c r="I60">
+        <v>0.82130000000000003</v>
+      </c>
+      <c r="J60">
+        <v>0.46729999999999999</v>
+      </c>
+      <c r="K60">
+        <v>0.92559999999999998</v>
+      </c>
+      <c r="L60">
+        <v>0.45040000000000002</v>
+      </c>
+      <c r="M60">
+        <v>0.96040000000000003</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B61" t="s">
+        <v>75</v>
+      </c>
+      <c r="D61">
+        <v>0.64890000000000003</v>
+      </c>
+      <c r="E61">
+        <v>0.93859999999999999</v>
+      </c>
+      <c r="F61">
+        <v>0.62849999999999995</v>
+      </c>
+      <c r="G61">
+        <v>0.81</v>
+      </c>
+      <c r="H61">
+        <v>0.68069999999999997</v>
+      </c>
+      <c r="I61">
+        <v>0.81810000000000005</v>
+      </c>
+      <c r="J61">
+        <v>0.5161</v>
+      </c>
+      <c r="K61">
+        <v>0.92290000000000005</v>
+      </c>
+      <c r="L61">
+        <v>0.50170000000000003</v>
+      </c>
+      <c r="M61">
+        <v>0.91559999999999997</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B62" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>